<commit_message>
added column for match results
</commit_message>
<xml_diff>
--- a/master_trades.xlsx
+++ b/master_trades.xlsx
@@ -8,9 +8,8 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markcarlebach/GolandProjects/camunda_initial/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{03F99C06-12B0-5340-81F1-FFEFF141F0B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="980" yWindow="2000" windowWidth="12900" windowHeight="17440" xr2:uid="{BB52BF36-742E-A141-9871-BA00098C4CD3}"/>
+    <workbookView xWindow="980" yWindow="2000" windowWidth="12900" windowHeight="17440"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t>tran_ref</t>
   </si>
@@ -83,13 +82,19 @@
   </si>
   <si>
     <t>Deliver</t>
+  </si>
+  <si>
+    <t>matched</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:ap="http://schemas.openxmlformats.org/officeDocument/2006/extended-properties" xmlns:op="http://schemas.openxmlformats.org/officeDocument/2006/custom-properties" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing" xmlns:comp="http://schemas.openxmlformats.org/drawingml/2006/compatibility" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:lc="http://schemas.openxmlformats.org/drawingml/2006/lockedCanvas" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:sl="http://schemas.openxmlformats.org/schemaLibrary/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xne="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mso="http://schemas.microsoft.com/office/2006/01/customui" xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:cppr="http://schemas.microsoft.com/office/2006/coverPageProps" xmlns:cdip="http://schemas.microsoft.com/office/2006/customDocumentInformationPanel" xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ntns="http://schemas.microsoft.com/office/2006/metadata/customXsn" xmlns:lp="http://schemas.microsoft.com/office/2006/metadata/longProperties" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" xmlns:msink="http://schemas.microsoft.com/ink/2010/main" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" xmlns:cdr14="http://schemas.microsoft.com/office/drawing/2010/chartDrawing" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:pic14="http://schemas.microsoft.com/office/drawing/2010/picture" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" xmlns:mso14="http://schemas.microsoft.com/office/2009/07/customui" xmlns:dgm14="http://schemas.microsoft.com/office/drawing/2010/diagram" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x12ac="http://schemas.microsoft.com/office/spreadsheetml/2011/1/ac" xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:xr4="http://schemas.microsoft.com/office/spreadsheetml/2016/revision4" xmlns:xr5="http://schemas.microsoft.com/office/spreadsheetml/2016/revision5" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr7="http://schemas.microsoft.com/office/spreadsheetml/2016/revision7" xmlns:xr8="http://schemas.microsoft.com/office/spreadsheetml/2016/revision8" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr11="http://schemas.microsoft.com/office/spreadsheetml/2016/revision11" xmlns:xr12="http://schemas.microsoft.com/office/spreadsheetml/2016/revision12" xmlns:xr13="http://schemas.microsoft.com/office/spreadsheetml/2016/revision13" xmlns:xr14="http://schemas.microsoft.com/office/spreadsheetml/2016/revision14" xmlns:xr15="http://schemas.microsoft.com/office/spreadsheetml/2016/revision15" xmlns:x16="http://schemas.microsoft.com/office/spreadsheetml/2014/11/main" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:mo="http://schemas.microsoft.com/office/mac/office/2008/main" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:v="urn:schemas-microsoft-com:vml" mc:Ignorable="c14 cdr14 a14 pic14 x14 xdr14 x14ac dsp mso14 dgm14 x15 x12ac x15ac xr xr2 xr3 xr4 xr5 xr6 xr7 xr8 xr9 xr10 xr11 xr12 xr13 xr14 xr15 x15 x16 x16r2 mo mx mv o v" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <fonts count="2">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -131,7 +136,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -440,18 +445,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF66005E-274A-2A41-87C2-712121E34C03}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="true" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="6" max="6" width="20.83203125" customWidth="1"/>
+    <col customWidth="true" max="6" min="6" width="20.83203125"/>
+    <col customWidth="true" max="8" min="7" width="17.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -470,8 +476,11 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -490,48 +499,54 @@
       <c r="F2">
         <v>1234</v>
       </c>
+      <c r="G2" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3">
         <v>987654</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D3">
         <v>145</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F3">
-        <v>1235</v>
+        <v>1234</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4">
         <v>987654</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D4">
         <v>145</v>
       </c>
       <c r="E4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F4">
-        <v>1234</v>
+        <v>1235</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -553,6 +568,7 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>